<commit_message>
Update Simulation Spaces and Real World Examples.xlsx
</commit_message>
<xml_diff>
--- a/Design and Notes/Simulation Spaces and Real World Examples.xlsx
+++ b/Design and Notes/Simulation Spaces and Real World Examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\Gravity-Sandbox\Design and Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2F1592C-D747-478F-A12D-135B42FA8847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6382EF-BE52-427B-AA19-EF6363640B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9360" yWindow="6030" windowWidth="27765" windowHeight="15105" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
   </bookViews>
@@ -144,7 +144,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +153,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -182,12 +198,18 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -507,7 +529,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,14 +539,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -722,6 +746,10 @@
       <c r="C36" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding physical constants and sizes to main spreadsheet
</commit_message>
<xml_diff>
--- a/Design and Notes/Simulation Spaces and Real World Examples.xlsx
+++ b/Design and Notes/Simulation Spaces and Real World Examples.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\Gravity-Sandbox\Design and Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6382EF-BE52-427B-AA19-EF6363640B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFDE518-925B-44C0-A577-3B83567E67BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="6030" windowWidth="27765" windowHeight="15105" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
+    <workbookView xWindow="7395" yWindow="1815" windowWidth="19365" windowHeight="15105" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Spaces" sheetId="2" r:id="rId1"/>
-    <sheet name="Astro Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Gravity" sheetId="3" r:id="rId1"/>
+    <sheet name="Spaces" sheetId="2" r:id="rId2"/>
+    <sheet name="Astro Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Original Sim Space</t>
   </si>
@@ -133,18 +134,243 @@
   </si>
   <si>
     <t>Body diameter default</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Gravitational_constant</t>
+  </si>
+  <si>
+    <t>m Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r Earth </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia Pro"/>
+        <family val="1"/>
+      </rPr>
+      <t>⊙</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">r </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia Pro"/>
+        <family val="1"/>
+      </rPr>
+      <t>⊙</t>
+    </r>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <r>
+      <t>GM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia Pro"/>
+        <family val="1"/>
+      </rPr>
+      <t>⊕</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia Pro"/>
+        <family val="1"/>
+      </rPr>
+      <t>⊙</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/kg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>•sec</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pc⋅M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>⊙</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>–1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>⋅(km/s)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>sec</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>ly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="174" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="176" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="180" formatCode="0.00000000000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +397,105 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Georgia Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Georgia Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202122"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +509,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,15 +517,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -210,10 +546,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="174" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -227,6 +582,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1276151</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A4D3CD-8FB7-4749-8CCD-36ED8089D963}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="504825" y="457200"/>
+          <a:ext cx="1590476" cy="704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,10 +929,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE3AE44-8D5D-43C2-B4A3-59984EC1FF62}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="13">
+        <v>6.6742999999999994E-11</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15">
+        <v>4.3009099999999998E-3</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="15">
+        <v>5.9722000000000002E+24</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="22">
+        <v>9460700000000000</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="13">
+        <v>3.0857E+16</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="14">
+        <v>3.2615599999999998</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="19">
+        <v>149597870700</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="20">
+        <v>1.32712440018E+20</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="20">
+        <v>398600441800000</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f>POWER(2, 1/3)</f>
+        <v>1.2599210498948732</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f>F27*F27</f>
+        <v>1.5874010519681996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f>F27*F28</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{B7FB08CD-1C3E-45E3-BA1B-7F65FF2818B4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1651B73-68FD-4429-9F74-D180E6E1C469}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -755,7 +1404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F03ABE-EB9B-4F5B-AAE8-3E2BB99A39EC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added buttons to control speed of simulation; More SimSpace refactoring
Simulation faster/slower buttons are not hooked up yet, need to add time base to core of simulation.
</commit_message>
<xml_diff>
--- a/Design and Notes/Simulation Spaces and Real World Examples.xlsx
+++ b/Design and Notes/Simulation Spaces and Real World Examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\Gravity-Sandbox\Design and Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFDE518-925B-44C0-A577-3B83567E67BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0379CF-E35E-4CD6-8ACC-7EA8B0B32A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="1815" windowWidth="19365" windowHeight="15105" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
+    <workbookView xWindow="7320" yWindow="3540" windowWidth="19365" windowHeight="15105" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
   </bookViews>
   <sheets>
     <sheet name="Gravity" sheetId="3" r:id="rId1"/>
@@ -364,11 +364,11 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="174" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="176" formatCode="0.0000000E+00"/>
-    <numFmt numFmtId="180" formatCode="0.00000000000E+00"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00000000000E+00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -540,29 +540,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -933,7 +933,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,203 +947,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="8"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>6.6742999999999994E-11</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13">
         <v>4.3009099999999998E-3</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="13">
         <v>5.9722000000000002E+24</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="20">
         <v>9460700000000000</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>3.0857E+16</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="14"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="12">
         <v>3.2615599999999998</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>149597870700</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="18">
         <v>1.32712440018E+20</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="18">
         <v>398600441800000</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="14"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27">
@@ -1188,16 +1188,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Added Big G to acceleration; Achieved stable earth orbit with ISS & Starlink!
FInished work in Issue #4 and got (LEO) earth orbit scenarios working properly using real values. Ran into a new issue with MEO and Geosynchronus orbits in this scenario, see new Issue #10 .
</commit_message>
<xml_diff>
--- a/Design and Notes/Simulation Spaces and Real World Examples.xlsx
+++ b/Design and Notes/Simulation Spaces and Real World Examples.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\Gravity-Sandbox\Design and Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0379CF-E35E-4CD6-8ACC-7EA8B0B32A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EDAC11-C88B-4F65-A9C5-D9979FC304DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3540" windowWidth="19365" windowHeight="15105" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
+    <workbookView xWindow="16140" yWindow="825" windowWidth="19365" windowHeight="15105" activeTab="1" xr2:uid="{46635536-B527-4D70-8D40-F00D32AA309B}"/>
   </bookViews>
   <sheets>
     <sheet name="Gravity" sheetId="3" r:id="rId1"/>
-    <sheet name="Spaces" sheetId="2" r:id="rId2"/>
-    <sheet name="Astro Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Orbits" sheetId="4" r:id="rId2"/>
+    <sheet name="Spaces" sheetId="2" r:id="rId3"/>
+    <sheet name="Astro Data" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Original Sim Space</t>
   </si>
@@ -354,13 +355,229 @@
   </si>
   <si>
     <t>ly</t>
+  </si>
+  <si>
+    <t>Unit Conversions</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <r>
+      <t>km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/kg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>•min</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sec</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>pc/m</t>
+  </si>
+  <si>
+    <t>kg/M sol</t>
+  </si>
+  <si>
+    <r>
+      <t>km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Orbit Altitude (km)</t>
+  </si>
+  <si>
+    <t>V (m/s)</t>
+  </si>
+  <si>
+    <t>V (Km/h)</t>
+  </si>
+  <si>
+    <t>Earth Orbits</t>
+  </si>
+  <si>
+    <t>ISS (5/25/2020)</t>
+  </si>
+  <si>
+    <t>Starlink</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Geosynchronous</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="10">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -369,8 +586,10 @@
     <numFmt numFmtId="167" formatCode="0.0000E+00"/>
     <numFmt numFmtId="168" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="169" formatCode="0.00000000000E+00"/>
+    <numFmt numFmtId="171" formatCode="0.000000000E+00"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +719,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -509,7 +736,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -526,15 +753,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -563,11 +800,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="5"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -622,6 +868,99 @@
         <a:xfrm>
           <a:off x="504825" y="457200"/>
           <a:ext cx="1590476" cy="704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1752381</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6FC76A-ADD2-4B99-924D-93F6CCB43465}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3448050" y="6505575"/>
+          <a:ext cx="1752381" cy="428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1076110</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47552</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023A6D0D-6B0A-4AD1-BDB9-087BF55A6762}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="533400" y="419100"/>
+          <a:ext cx="1723810" cy="580952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -930,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE3AE44-8D5D-43C2-B4A3-59984EC1FF62}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,8 +1323,12 @@
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="15">
+        <v>6371</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -1145,13 +1488,49 @@
       <c r="F21" s="19"/>
       <c r="G21" s="12"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="25">
+        <f>B8</f>
+        <v>6.6742999999999994E-11</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>POWER(1/1000,3)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="F27">
         <f>POWER(2, 1/3)</f>
         <v>1.2599210498948732</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f>POWER(60,2)</f>
+        <v>3600</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="F28">
         <f>F27*F27</f>
         <v>1.5874010519681996</v>
@@ -1161,6 +1540,59 @@
       <c r="F29">
         <f>F27*F28</f>
         <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="B30" s="25">
+        <f>B26*B27*B28</f>
+        <v>2.4027479999999998E-16</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="25">
+        <f>B26</f>
+        <v>6.6742999999999994E-11</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f>1/30860000000000000</f>
+        <v>3.2404406999351912E-17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="26">
+        <v>1.9889999999999999E+30</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f>POWER(1/1000,2)</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="25">
+        <f>B32*B33*B34*B35</f>
+        <v>4.3017442320155532E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1174,6 +1606,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FD0F7-5641-4B82-B36B-D8B42B40CABB}">
+  <dimension ref="A7:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="27">
+        <v>398600441800000</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="15">
+        <v>6371</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>420</v>
+      </c>
+      <c r="B13" s="28">
+        <f>SQRT(B$8/((B$9+A13)*1000))</f>
+        <v>7661.2921308240902</v>
+      </c>
+      <c r="C13" s="29">
+        <f>B13*3600/1000</f>
+        <v>27580.651670966727</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>550</v>
+      </c>
+      <c r="B14" s="28">
+        <f t="shared" ref="B14:B16" si="0">SQRT(B$8/((B$9+A14)*1000))</f>
+        <v>7588.9984345948578</v>
+      </c>
+      <c r="C14" s="29">
+        <f t="shared" ref="C14:C16" si="1">B14*3600/1000</f>
+        <v>27320.394364541491</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>20180</v>
+      </c>
+      <c r="B15" s="28">
+        <f t="shared" si="0"/>
+        <v>3874.6140281191451</v>
+      </c>
+      <c r="C15" s="29">
+        <f t="shared" si="1"/>
+        <v>13948.610501228923</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>35786</v>
+      </c>
+      <c r="B16" s="28">
+        <f t="shared" si="0"/>
+        <v>3074.9215415063541</v>
+      </c>
+      <c r="C16" s="29">
+        <f t="shared" si="1"/>
+        <v>11069.717549422876</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="31">
+        <f>2*PI()*(A14+B9)</f>
+        <v>43485.925510989917</v>
+      </c>
+      <c r="C23" s="30">
+        <f>C13-C14</f>
+        <v>260.25730642523558</v>
+      </c>
+      <c r="D23">
+        <f>B23/C23</f>
+        <v>167.08820247274085</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>D23/4</f>
+        <v>41.772050618185212</v>
+      </c>
+      <c r="E24">
+        <f>D24*60</f>
+        <v>2506.3230370911128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1651B73-68FD-4429-9F74-D180E6E1C469}">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -1404,7 +1984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F03ABE-EB9B-4F5B-AAE8-3E2BB99A39EC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>